<commit_message>
Modification on session page (dropdown not editable) - cleaning of the code
</commit_message>
<xml_diff>
--- a/code/flask-server/download/Calendar_-Na0vd-EA6ks5SxdM3XP.xlsx
+++ b/code/flask-server/download/Calendar_-Na0vd-EA6ks5SxdM3XP.xlsx
@@ -507,7 +507,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2023-07-07</t>
+          <t>2023-07-05</t>
         </is>
       </c>
     </row>
@@ -550,31 +550,31 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2023-07-12</t>
+          <t>2023-07-10</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ELT</t>
+          <t>ATM</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>85754</t>
+          <t>85743</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>FONDAMENTI DI ROBOTICA</t>
+          <t>SISTEMI INFORMATICI</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -583,7 +583,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Zanchettin Andrea Maria-Rocco Paolo</t>
+          <t>Gatti Nicola-Mottola Luca</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -600,24 +600,24 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ELT</t>
+          <t>ATM</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>85754</t>
+          <t>85743</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>FONDAMENTI DI ROBOTICA</t>
+          <t>SISTEMI INFORMATICI</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -626,7 +626,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Zanchettin Andrea Maria-Rocco Paolo</t>
+          <t>Gatti Nicola-Mottola Luca</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -722,7 +722,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>2023-07-12</t>
+          <t>2023-07-13</t>
         </is>
       </c>
     </row>
@@ -815,24 +815,24 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ATM</t>
+          <t>ELT</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>85743</t>
+          <t>85754</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>SISTEMI INFORMATICI</t>
+          <t>FONDAMENTI DI ROBOTICA</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -841,7 +841,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Gatti Nicola-Mottola Luca</t>
+          <t>Zanchettin Andrea Maria-Rocco Paolo</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -851,31 +851,31 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>2023-07-05</t>
+          <t>2023-07-03</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ATM</t>
+          <t>ELT</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>85743</t>
+          <t>85754</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>SISTEMI INFORMATICI</t>
+          <t>FONDAMENTI DI ROBOTICA</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -884,7 +884,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Gatti Nicola-Mottola Luca</t>
+          <t>Zanchettin Andrea Maria-Rocco Paolo</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -894,7 +894,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>2023-07-10</t>
+          <t>2023-07-08</t>
         </is>
       </c>
     </row>
@@ -937,7 +937,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>2023-07-06</t>
+          <t>2023-07-04</t>
         </is>
       </c>
     </row>
@@ -980,7 +980,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>2023-07-13</t>
+          <t>2023-07-12</t>
         </is>
       </c>
     </row>

</xml_diff>